<commit_message>
add required and readonly parser
</commit_message>
<xml_diff>
--- a/test/fixture/question_types.xlsx
+++ b/test/fixture/question_types.xlsx
@@ -59,7 +59,7 @@
     <t>my_string</t>
   </si>
   <si>
-    <t>Text </t>
+    <t>Text</t>
   </si>
   <si>
     <t>Can be short or long but always one line (type = text)</t>
@@ -80,7 +80,7 @@
     <t>my_int</t>
   </si>
   <si>
-    <t>Integer </t>
+    <t>Integer</t>
   </si>
   <si>
     <t>For this field (type=integer)</t>
@@ -92,7 +92,7 @@
     <t>my_decimal</t>
   </si>
   <si>
-    <t>Decimal </t>
+    <t>Decimal</t>
   </si>
   <si>
     <t>For this field (type=decimal)</t>
@@ -110,7 +110,7 @@
     <t>my_date</t>
   </si>
   <si>
-    <t>Date </t>
+    <t>Date</t>
   </si>
   <si>
     <t>For this field (type=date)</t>
@@ -122,7 +122,7 @@
     <t>my_time</t>
   </si>
   <si>
-    <t>Time </t>
+    <t>Time</t>
   </si>
   <si>
     <t>Times are easy! (type=time)</t>
@@ -131,7 +131,7 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>Date and time </t>
+    <t>Date and time</t>
   </si>
   <si>
     <t>For exact times, will be converted to UTC/GMT (type=dateTime)</t>
@@ -176,7 +176,7 @@
     <t>my_geopoint</t>
   </si>
   <si>
-    <t>Geopoint </t>
+    <t>Geopoint</t>
   </si>
   <si>
     <t>This will record the gps location. (type=geopoint)</t>
@@ -573,8 +573,8 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -668,7 +668,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="8.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>